<commit_message>
Calculated vote prediction accuracy using RMSE for color hist and IncV3 notebooks
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08218420-9F68-4A6E-9828-957D18D35E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772B2636-E886-4090-932E-C66107502E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8775" yWindow="1260" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,6 +761,18 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
+      <c r="B15">
+        <v>4.42</v>
+      </c>
+      <c r="C15">
+        <v>4.51</v>
+      </c>
+      <c r="D15">
+        <v>4.51</v>
+      </c>
+      <c r="E15">
+        <v>4.51</v>
+      </c>
       <c r="G15" t="s">
         <v>4</v>
       </c>
@@ -769,6 +781,18 @@
       <c r="A16" t="s">
         <v>5</v>
       </c>
+      <c r="B16">
+        <v>4.47</v>
+      </c>
+      <c r="C16">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="D16">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E16">
+        <v>4.6100000000000003</v>
+      </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
@@ -793,6 +817,18 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
+      <c r="B19">
+        <v>4.08</v>
+      </c>
+      <c r="C19">
+        <v>4.24</v>
+      </c>
+      <c r="D19">
+        <v>4.34</v>
+      </c>
+      <c r="E19">
+        <v>4.4400000000000004</v>
+      </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
@@ -800,6 +836,18 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>4.2</v>
+      </c>
+      <c r="D20">
+        <v>4.47</v>
+      </c>
+      <c r="E20">
+        <v>4.5</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added RMSE and Manhattan evaluation to instance-based vote count prediction (only InceptionV3 and color hist included)
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772B2636-E886-4090-932E-C66107502E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04B5A90-7354-4ED9-9FC8-97F407502B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="1260" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8760" yWindow="1485" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>k=1</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>BASADO EN INSTANCIAS</t>
+  </si>
+  <si>
+    <t>k=15</t>
+  </si>
+  <si>
+    <t>k=20</t>
   </si>
 </sst>
 </file>
@@ -108,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,50 +400,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -468,7 +475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -506,7 +513,7 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -544,7 +551,7 @@
         <v>6.68</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -582,7 +589,7 @@
         <v>5.91</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -620,7 +627,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -658,7 +665,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -696,42 +703,42 @@
         <v>5.82</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -756,8 +763,17 @@
       <c r="K14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -776,8 +792,29 @@
       <c r="G15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>6.03</v>
+      </c>
+      <c r="I15">
+        <v>4.93</v>
+      </c>
+      <c r="J15">
+        <v>4.66</v>
+      </c>
+      <c r="K15">
+        <v>4.54</v>
+      </c>
+      <c r="L15">
+        <v>4.51</v>
+      </c>
+      <c r="M15">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="N15">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -796,8 +833,29 @@
       <c r="G16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>6.08</v>
+      </c>
+      <c r="I16">
+        <v>4.92</v>
+      </c>
+      <c r="J16">
+        <v>4.71</v>
+      </c>
+      <c r="K16">
+        <v>4.57</v>
+      </c>
+      <c r="L16">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="M16">
+        <v>4.43</v>
+      </c>
+      <c r="N16">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -805,7 +863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -813,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -832,8 +890,29 @@
       <c r="G19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>5.36</v>
+      </c>
+      <c r="I19">
+        <v>4.32</v>
+      </c>
+      <c r="J19">
+        <v>4.13</v>
+      </c>
+      <c r="K19">
+        <v>4.07</v>
+      </c>
+      <c r="L19">
+        <v>3.98</v>
+      </c>
+      <c r="M19">
+        <v>4.05</v>
+      </c>
+      <c r="N19">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -851,6 +930,27 @@
       </c>
       <c r="G20" t="s">
         <v>9</v>
+      </c>
+      <c r="H20">
+        <v>5.6</v>
+      </c>
+      <c r="I20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J20">
+        <v>4.24</v>
+      </c>
+      <c r="K20">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="L20">
+        <v>4.08</v>
+      </c>
+      <c r="M20">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new notebook type: VCP prediction using feat prototypes, not only vote prototypes
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04B5A90-7354-4ED9-9FC8-97F407502B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A910DC-C724-4722-AAD6-D832CEFECE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="1485" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="855" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>k=1</t>
   </si>
@@ -79,6 +80,9 @@
   </si>
   <si>
     <t>k=20</t>
+  </si>
+  <si>
+    <t>BASADO EN PRTS (Promedio de características)</t>
   </si>
 </sst>
 </file>
@@ -400,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -425,7 +429,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -443,7 +447,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -475,7 +479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +517,7 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -551,7 +555,7 @@
         <v>6.68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -589,7 +593,7 @@
         <v>5.91</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -627,7 +631,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -665,7 +669,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -703,7 +707,7 @@
         <v>5.82</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -719,8 +723,11 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -737,8 +744,26 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U13" t="s">
+        <v>11</v>
+      </c>
+      <c r="V13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -773,7 +798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -814,7 +839,7 @@
         <v>4.43</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -855,7 +880,7 @@
         <v>4.3899999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -863,7 +888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -871,7 +896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -911,8 +936,29 @@
       <c r="N19">
         <v>4.07</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>4.91</v>
+      </c>
+      <c r="R19">
+        <v>4.55</v>
+      </c>
+      <c r="S19">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="T19">
+        <v>4.72</v>
+      </c>
+      <c r="U19">
+        <v>4.57</v>
+      </c>
+      <c r="V19">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -964,4 +1010,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B7C08-E906-4552-8C8D-E0573F7814FB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tested general VCP notebook with different feat- types and sim. metrics
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A910DC-C724-4722-AAD6-D832CEFECE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDEE974-5421-4F83-9B85-BD9C915FBF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="855" windowWidth="11070" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9150" yWindow="465" windowWidth="11070" windowHeight="9705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Cluster-Based" sheetId="2" r:id="rId2"/>
+    <sheet name="KNN(Instance-based)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>k=1</t>
   </si>
@@ -83,14 +84,49 @@
   </si>
   <si>
     <t>BASADO EN PRTS (Promedio de características)</t>
+  </si>
+  <si>
+    <t>k=10</t>
+  </si>
+  <si>
+    <t>INV3-EUCLID</t>
+  </si>
+  <si>
+    <t>INV3-COSINE</t>
+  </si>
+  <si>
+    <t>HIST-COSINE</t>
+  </si>
+  <si>
+    <t>BASADO EN PRTS. PROMEDIADOS DE CARACTERÍSTICAS</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>MICROSEGUNDOS</t>
+  </si>
+  <si>
+    <t>INV1-EUCLID</t>
+  </si>
+  <si>
+    <t>INV3-COS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -406,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,9 +762,6 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="Q12" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -744,24 +780,15 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="Q13" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>1</v>
-      </c>
-      <c r="S13" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" t="s">
-        <v>3</v>
-      </c>
-      <c r="U13" t="s">
-        <v>11</v>
-      </c>
-      <c r="V13" t="s">
-        <v>12</v>
-      </c>
+      <c r="P13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -797,6 +824,24 @@
       <c r="N14" t="s">
         <v>17</v>
       </c>
+      <c r="Q14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T14" t="s">
+        <v>3</v>
+      </c>
+      <c r="U14" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1000,7 +1045,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="P13:V13"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:M2"/>
@@ -1014,6 +1060,302 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B7C08-E906-4552-8C8D-E0573F7814FB}">
+  <dimension ref="A1:P19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="C4">
+        <v>4.28</v>
+      </c>
+      <c r="D4">
+        <v>4.47</v>
+      </c>
+      <c r="E4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="F4">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>4.05</v>
+      </c>
+      <c r="C5">
+        <v>4.3</v>
+      </c>
+      <c r="D5">
+        <v>4.42</v>
+      </c>
+      <c r="E5">
+        <v>4.46</v>
+      </c>
+      <c r="F5">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4.42</v>
+      </c>
+      <c r="C6">
+        <v>4.51</v>
+      </c>
+      <c r="D6">
+        <v>4.51</v>
+      </c>
+      <c r="E6">
+        <v>4.51</v>
+      </c>
+      <c r="F6">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4.47</v>
+      </c>
+      <c r="C7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="D7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="F7">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>1613</v>
+      </c>
+      <c r="C12">
+        <v>1256</v>
+      </c>
+      <c r="D12">
+        <v>1014</v>
+      </c>
+      <c r="E12">
+        <v>1054</v>
+      </c>
+      <c r="F12">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>1091</v>
+      </c>
+      <c r="C13">
+        <v>1081</v>
+      </c>
+      <c r="D13">
+        <v>1187</v>
+      </c>
+      <c r="E13">
+        <v>1288</v>
+      </c>
+      <c r="F13">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>445</v>
+      </c>
+      <c r="C14">
+        <v>484</v>
+      </c>
+      <c r="D14">
+        <v>441</v>
+      </c>
+      <c r="E14">
+        <v>468</v>
+      </c>
+      <c r="F14">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>478</v>
+      </c>
+      <c r="C15">
+        <v>450</v>
+      </c>
+      <c r="D15">
+        <v>463</v>
+      </c>
+      <c r="E15">
+        <v>463</v>
+      </c>
+      <c r="F15">
+        <v>474</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF44FBB3-3904-4DD5-9CD9-648DAB53717C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Implemented general instance-based VCP notebook
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDEE974-5421-4F83-9B85-BD9C915FBF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FD8DDD-AE6E-4A96-B24B-6F5BC1FD220C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="465" windowWidth="11070" windowHeight="9705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8100" yWindow="960" windowWidth="12060" windowHeight="9705" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
   <si>
     <t>k=1</t>
   </si>
@@ -92,12 +92,6 @@
     <t>INV3-EUCLID</t>
   </si>
   <si>
-    <t>INV3-COSINE</t>
-  </si>
-  <si>
-    <t>HIST-COSINE</t>
-  </si>
-  <si>
     <t>BASADO EN PRTS. PROMEDIADOS DE CARACTERÍSTICAS</t>
   </si>
   <si>
@@ -111,6 +105,9 @@
   </si>
   <si>
     <t>INV3-COS</t>
+  </si>
+  <si>
+    <t>BASADO EN KNN TRADICIONAL (INSTANCIA A INSTANCIA)</t>
   </si>
 </sst>
 </file>
@@ -1060,17 +1057,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B7C08-E906-4552-8C8D-E0573F7814FB}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1078,9 +1075,9 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1088,7 +1085,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1125,9 +1122,9 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>4.05</v>
@@ -1145,7 +1142,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1165,7 +1162,7 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1185,19 +1182,19 @@
         <v>4.6100000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1205,7 +1202,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1242,9 +1239,9 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>1091</v>
@@ -1262,7 +1259,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1301,46 +1298,15 @@
       <c r="F15">
         <v>474</v>
       </c>
-      <c r="L15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1356,12 +1322,214 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF44FBB3-3904-4DD5-9CD9-648DAB53717C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>5.26</v>
+      </c>
+      <c r="C4">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="D4">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4.09</v>
+      </c>
+      <c r="F4">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>5.58</v>
+      </c>
+      <c r="C5">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="D5">
+        <v>4.26</v>
+      </c>
+      <c r="E5">
+        <v>4.07</v>
+      </c>
+      <c r="F5">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>8915</v>
+      </c>
+      <c r="C12">
+        <v>8764</v>
+      </c>
+      <c r="D12">
+        <v>8976</v>
+      </c>
+      <c r="E12">
+        <v>9000</v>
+      </c>
+      <c r="F12">
+        <v>9390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>11178</v>
+      </c>
+      <c r="C13">
+        <v>11529</v>
+      </c>
+      <c r="D13">
+        <v>11677</v>
+      </c>
+      <c r="E13">
+        <v>11669</v>
+      </c>
+      <c r="F13">
+        <v>11557</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A10:I10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tested different feat. types and sim. metrics on the instance-based VCP notebook
</commit_message>
<xml_diff>
--- a/results/vcp-results.xlsx
+++ b/results/vcp-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastián\Desktop\MLStuff\xai-ucm-unsup\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FD8DDD-AE6E-4A96-B24B-6F5BC1FD220C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C2C172-5333-4DD8-B2D7-599BE7EB2AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="960" windowWidth="12060" windowHeight="9705" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF44FBB3-3904-4DD5-9CD9-648DAB53717C}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,10 +1417,40 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>6.3</v>
+      </c>
+      <c r="C6">
+        <v>4.99</v>
+      </c>
+      <c r="D6">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E6">
+        <v>4.55</v>
+      </c>
+      <c r="F6">
+        <v>4.41</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6.39</v>
+      </c>
+      <c r="C7">
+        <v>5.04</v>
+      </c>
+      <c r="D7">
+        <v>4.7</v>
+      </c>
+      <c r="E7">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="F7">
+        <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1507,10 +1537,40 @@
       <c r="A14" t="s">
         <v>4</v>
       </c>
+      <c r="B14">
+        <v>3783</v>
+      </c>
+      <c r="C14">
+        <v>3957</v>
+      </c>
+      <c r="D14">
+        <v>3938</v>
+      </c>
+      <c r="E14">
+        <v>4337</v>
+      </c>
+      <c r="F14">
+        <v>5182</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
+      </c>
+      <c r="B15">
+        <v>6934</v>
+      </c>
+      <c r="C15">
+        <v>6944</v>
+      </c>
+      <c r="D15">
+        <v>7056</v>
+      </c>
+      <c r="E15">
+        <v>7368</v>
+      </c>
+      <c r="F15">
+        <v>8232</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>